<commit_message>
in progress adding GSK_LAYOUT_COMPLIANCE_SEQUENCE
</commit_message>
<xml_diff>
--- a/Projects/PSAPAC_SAND3/Data/gskau_external_target.xlsx
+++ b/Projects/PSAPAC_SAND3/Data/gskau_external_target.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Secondary_Display" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="162">
   <si>
     <t xml:space="preserve">Store Number</t>
   </si>
@@ -436,6 +436,18 @@
   </si>
   <si>
     <t xml:space="preserve">Panadol Base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
   </si>
   <si>
     <t xml:space="preserve">Section</t>
@@ -599,7 +611,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF950E"/>
       </patternFill>
     </fill>
     <fill>
@@ -1176,9 +1188,9 @@
       <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFAECF00"/>
       <rgbColor rgb="FFFFC000"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF950E"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFA6A6A6"/>
@@ -1208,14 +1220,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="34.0647773279352"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="34.3846153846154"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.10526315789474"/>
@@ -1418,21 +1430,21 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="6" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="6" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="6" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="41.5627530364373"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="6" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="6" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="6" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="6" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="6" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="6" width="9.10526315789474"/>
   </cols>
@@ -5549,19 +5561,19 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="48" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="48" width="33.1012145748988"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="48" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="48" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="48" width="36.6356275303644"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="48" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="48" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="48" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="49" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="49" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="50" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="50" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="50" width="9.10526315789474"/>
@@ -5934,23 +5946,24 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFF950E"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.2429149797571"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.6356275303644"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
@@ -6328,19 +6341,20 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.0971659919028"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.0404858299595"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.4534412955466"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.5303643724696"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="49" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="49" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="49" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="49" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -6698,16 +6712,16 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.6315789473684"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.0607287449393"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="49" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.1417004048583"/>
@@ -7029,23 +7043,24 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFAECF00"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5991902834008"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.1943319838057"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.9473684210526"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -7382,6 +7397,26 @@
         <v>43876</v>
       </c>
       <c r="J11" s="63"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7409,21 +7444,21 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="6" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="6" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="6" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="40.919028340081"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="6" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="6" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="6" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="6" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="6" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="6" width="9.10526315789474"/>
   </cols>
@@ -9520,7 +9555,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>40</v>
@@ -10136,7 +10171,7 @@
         <v>78</v>
       </c>
       <c r="K20" s="31" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="L20" s="31"/>
       <c r="M20" s="31" t="s">
@@ -10178,7 +10213,7 @@
         <v>79</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="L21" s="32" t="s">
         <v>54</v>
@@ -10961,16 +10996,16 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="6" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="9" min="2" style="6" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="10" style="6" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="64" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="64" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="64" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="6" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="65" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -10984,7 +11019,7 @@
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="66" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
@@ -10997,7 +11032,7 @@
     <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="66" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C3" s="66"/>
       <c r="D3" s="66"/>
@@ -11020,7 +11055,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="68" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B5" s="69"/>
       <c r="C5" s="69"/>
@@ -11033,7 +11068,7 @@
     </row>
     <row r="6" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="70" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B6" s="70" t="s">
         <v>55</v>
@@ -11065,28 +11100,28 @@
         <v>8</v>
       </c>
       <c r="B7" s="72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C7" s="72" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D7" s="73" t="s">
         <v>128</v>
       </c>
       <c r="E7" s="73" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F7" s="73" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G7" s="73" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H7" s="73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="I7" s="73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11094,28 +11129,28 @@
         <v>9</v>
       </c>
       <c r="B8" s="72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C8" s="72" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D8" s="73" t="s">
         <v>128</v>
       </c>
       <c r="E8" s="73" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F8" s="73" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G8" s="73" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H8" s="73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="I8" s="73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11123,28 +11158,28 @@
         <v>10</v>
       </c>
       <c r="B9" s="72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C9" s="72" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D9" s="73" t="s">
         <v>128</v>
       </c>
       <c r="E9" s="73" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F9" s="73" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G9" s="73" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H9" s="73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="I9" s="73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11152,28 +11187,28 @@
         <v>11</v>
       </c>
       <c r="B10" s="72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C10" s="72" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D10" s="73" t="s">
         <v>128</v>
       </c>
       <c r="E10" s="73" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F10" s="73" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G10" s="73" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H10" s="73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="I10" s="73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11181,28 +11216,28 @@
         <v>12</v>
       </c>
       <c r="B11" s="72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C11" s="72" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D11" s="73" t="s">
         <v>128</v>
       </c>
       <c r="E11" s="73" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F11" s="73" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G11" s="73" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H11" s="73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="I11" s="73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11214,7 +11249,7 @@
     </row>
     <row r="13" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="70" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B13" s="70" t="s">
         <v>71</v>
@@ -11234,16 +11269,16 @@
         <v>8</v>
       </c>
       <c r="B14" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="72" t="s">
         <v>150</v>
-      </c>
-      <c r="C14" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="D14" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="E14" s="72" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11251,16 +11286,16 @@
         <v>9</v>
       </c>
       <c r="B15" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="72" t="s">
         <v>150</v>
-      </c>
-      <c r="C15" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="D15" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="E15" s="72" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11268,16 +11303,16 @@
         <v>10</v>
       </c>
       <c r="B16" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="D16" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" s="72" t="s">
         <v>150</v>
-      </c>
-      <c r="C16" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="D16" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="E16" s="72" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11285,16 +11320,16 @@
         <v>11</v>
       </c>
       <c r="B17" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="72" t="s">
         <v>150</v>
-      </c>
-      <c r="C17" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="E17" s="72" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11302,16 +11337,16 @@
         <v>12</v>
       </c>
       <c r="B18" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" s="72" t="s">
         <v>150</v>
-      </c>
-      <c r="C18" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="D18" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="72" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11322,7 +11357,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="68" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B20" s="0"/>
       <c r="C20" s="0"/>
@@ -11330,7 +11365,7 @@
     </row>
     <row r="21" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="70" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B21" s="70" t="s">
         <v>78</v>
@@ -11348,7 +11383,7 @@
         <v>128</v>
       </c>
       <c r="C22" s="72" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D22" s="0"/>
     </row>
@@ -11360,7 +11395,7 @@
         <v>128</v>
       </c>
       <c r="C23" s="72" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D23" s="0"/>
     </row>
@@ -11372,7 +11407,7 @@
         <v>128</v>
       </c>
       <c r="C24" s="72" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D24" s="0"/>
     </row>
@@ -11384,7 +11419,7 @@
         <v>128</v>
       </c>
       <c r="C25" s="72" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D25" s="0"/>
     </row>
@@ -11396,7 +11431,7 @@
         <v>128</v>
       </c>
       <c r="C26" s="72" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D26" s="0"/>
     </row>
@@ -11416,10 +11451,10 @@
     </row>
     <row r="29" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="70" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B29" s="70" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C29" s="70" t="s">
         <v>83</v>
@@ -11439,7 +11474,7 @@
         <v>128</v>
       </c>
       <c r="D30" s="72" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11453,7 +11488,7 @@
         <v>128</v>
       </c>
       <c r="D31" s="72" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11467,7 +11502,7 @@
         <v>128</v>
       </c>
       <c r="D32" s="72" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11481,7 +11516,7 @@
         <v>128</v>
       </c>
       <c r="D33" s="72" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11495,7 +11530,7 @@
         <v>128</v>
       </c>
       <c r="D34" s="72" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11506,7 +11541,7 @@
     </row>
     <row r="36" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="68" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B36" s="0"/>
       <c r="C36" s="0"/>
@@ -11514,16 +11549,16 @@
     </row>
     <row r="37" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="70" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B37" s="70" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C37" s="70" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D37" s="70" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11531,13 +11566,13 @@
         <v>8</v>
       </c>
       <c r="B38" s="72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C38" s="72" t="s">
         <v>128</v>
       </c>
       <c r="D38" s="72" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11545,13 +11580,13 @@
         <v>9</v>
       </c>
       <c r="B39" s="72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C39" s="72" t="s">
         <v>128</v>
       </c>
       <c r="D39" s="72" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11559,13 +11594,13 @@
         <v>10</v>
       </c>
       <c r="B40" s="72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C40" s="72" t="s">
         <v>128</v>
       </c>
       <c r="D40" s="72" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11573,13 +11608,13 @@
         <v>11</v>
       </c>
       <c r="B41" s="72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C41" s="72" t="s">
         <v>128</v>
       </c>
       <c r="D41" s="72" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11587,13 +11622,13 @@
         <v>12</v>
       </c>
       <c r="B42" s="72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C42" s="72" t="s">
         <v>128</v>
       </c>
       <c r="D42" s="72" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update target col names
</commit_message>
<xml_diff>
--- a/Projects/PSAPAC_SAND3/Data/gskau_external_target.xlsx
+++ b/Projects/PSAPAC_SAND3/Data/gskau_external_target.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Secondary_Display" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="171">
   <si>
     <t xml:space="preserve">Store Number</t>
   </si>
@@ -351,12 +351,15 @@
     <t xml:space="preserve">KPI Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Store Banner</t>
+    <t xml:space="preserve">Store Banner (static.stores =&gt; additional_attribute_20)</t>
   </si>
   <si>
     <t xml:space="preserve">Sub Category</t>
   </si>
   <si>
+    <t xml:space="preserve">Super Brand (label in product table)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stacking</t>
   </si>
   <si>
@@ -366,6 +369,9 @@
     <t xml:space="preserve">GSK_LAYOUT_COMPLIANCE_BLOCK </t>
   </si>
   <si>
+    <t xml:space="preserve">TWC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pain Main Shelf, Pain Main Shelf - Grcy</t>
   </si>
   <si>
@@ -378,7 +384,7 @@
     <t xml:space="preserve">Toothpaste</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-TerryWhite</t>
+    <t xml:space="preserve">Non-TWC</t>
   </si>
   <si>
     <t xml:space="preserve">SOS Threshold %</t>
@@ -390,7 +396,19 @@
     <t xml:space="preserve">GSK_LAYOUT_COMPLIANCE_BRAND_FSOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Wellness Main Shelf, Wellness Main Shelf - Grcy</t>
+    <t xml:space="preserve">Pain Main Shelf, Wellness Main Shelf, Pain Main Shelf - Grcy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicorette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panadol Base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pain Main Shelf, Wellness Main Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panadol Night</t>
   </si>
   <si>
     <t xml:space="preserve">Target %</t>
@@ -427,9 +445,6 @@
   </si>
   <si>
     <t xml:space="preserve">GSK_LAYOUT_COMPLIANCE_SEQUENCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TWC</t>
   </si>
   <si>
     <t xml:space="preserve">Nurofen</t>
@@ -849,7 +864,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1066,6 +1081,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1082,10 +1101,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1098,12 +1113,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1226,20 +1245,20 @@
   </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="2" sqref="B2 B26 L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="35.2429149797571"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="37.8137651821862"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.10526315789474"/>
@@ -1435,7 +1454,7 @@
   <dimension ref="1:56"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+      <selection pane="topLeft" activeCell="C40" activeCellId="2" sqref="B2 B26 C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1443,19 +1462,19 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="6" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="6" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="6" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="28.2793522267206"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="6" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="46.2753036437247"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="6" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="6" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="6" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="6" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="6" width="9.10526315789474"/>
@@ -5573,19 +5592,19 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="1" sqref="B2 B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="48" width="34.3846153846154"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="48" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="48" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="48" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="48" width="55.4858299595142"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="48" width="40.5991902834008"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="48" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="48" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="48" width="36.5263157894737"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="48" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="49" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="49" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="50" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="50" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="50" width="9.10526315789474"/>
@@ -5595,7 +5614,7 @@
       <c r="A1" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>107</v>
       </c>
       <c r="C1" s="51" t="s">
@@ -5605,13 +5624,13 @@
         <v>108</v>
       </c>
       <c r="E1" s="52" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H1" s="51" t="s">
         <v>11</v>
@@ -5622,13 +5641,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>49</v>
+        <v>112</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>113</v>
       </c>
       <c r="C2" s="53" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D2" s="53" t="s">
         <v>51</v>
@@ -5637,25 +5656,25 @@
         <v>52</v>
       </c>
       <c r="F2" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G2" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G2" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H2" s="55" t="n">
+      <c r="H2" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I2" s="56"/>
+      <c r="I2" s="57"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="53" t="s">
-        <v>49</v>
+        <v>112</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>113</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D3" s="53" t="s">
         <v>51</v>
@@ -5664,25 +5683,25 @@
         <v>59</v>
       </c>
       <c r="F3" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G3" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G3" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H3" s="55" t="n">
+      <c r="H3" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I3" s="56"/>
+      <c r="I3" s="57"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="53" t="s">
-        <v>49</v>
+        <v>112</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>113</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D4" s="53" t="s">
         <v>93</v>
@@ -5691,25 +5710,25 @@
         <v>52</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G4" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G4" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H4" s="55" t="n">
+      <c r="H4" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I4" s="56"/>
+      <c r="I4" s="57"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="53" t="s">
-        <v>49</v>
+        <v>112</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>113</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D5" s="53" t="s">
         <v>77</v>
@@ -5718,52 +5737,52 @@
         <v>59</v>
       </c>
       <c r="F5" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G5" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H5" s="55" t="n">
+      <c r="H5" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I5" s="56"/>
+      <c r="I5" s="57"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="53" t="s">
-        <v>49</v>
+        <v>112</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>113</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D6" s="53" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E6" s="53" t="s">
         <v>81</v>
       </c>
       <c r="F6" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G6" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H6" s="55" t="n">
+      <c r="H6" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I6" s="57"/>
+      <c r="I6" s="58"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" s="53" t="s">
-        <v>49</v>
+        <v>112</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>113</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D7" s="53" t="s">
         <v>86</v>
@@ -5772,25 +5791,25 @@
         <v>52</v>
       </c>
       <c r="F7" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G7" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G7" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H7" s="55" t="n">
+      <c r="H7" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I7" s="57"/>
+      <c r="I7" s="58"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="53" t="s">
-        <v>116</v>
+        <v>112</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>118</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D8" s="53" t="s">
         <v>51</v>
@@ -5799,25 +5818,25 @@
         <v>52</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G8" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G8" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H8" s="55" t="n">
+      <c r="H8" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I8" s="57"/>
+      <c r="I8" s="58"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="53" t="s">
-        <v>116</v>
+        <v>112</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>118</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D9" s="53" t="s">
         <v>51</v>
@@ -5826,25 +5845,25 @@
         <v>59</v>
       </c>
       <c r="F9" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G9" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H9" s="55" t="n">
+      <c r="H9" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I9" s="57"/>
+      <c r="I9" s="58"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>116</v>
+        <v>112</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>118</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D10" s="53" t="s">
         <v>93</v>
@@ -5853,25 +5872,25 @@
         <v>52</v>
       </c>
       <c r="F10" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G10" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G10" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H10" s="55" t="n">
+      <c r="H10" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I10" s="57"/>
+      <c r="I10" s="58"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" s="53" t="s">
-        <v>116</v>
+        <v>112</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>118</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D11" s="53" t="s">
         <v>77</v>
@@ -5880,52 +5899,52 @@
         <v>59</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G11" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G11" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H11" s="55" t="n">
+      <c r="H11" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I11" s="57"/>
+      <c r="I11" s="58"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="53" t="s">
-        <v>114</v>
-      </c>
       <c r="D12" s="53" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E12" s="53" t="s">
         <v>81</v>
       </c>
       <c r="F12" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G12" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G12" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H12" s="55" t="n">
+      <c r="H12" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I12" s="57"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="C13" s="53" t="s">
-        <v>114</v>
       </c>
       <c r="D13" s="53" t="s">
         <v>86</v>
@@ -5934,15 +5953,15 @@
         <v>52</v>
       </c>
       <c r="F13" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G13" s="54" t="n">
+        <v>115</v>
+      </c>
+      <c r="G13" s="55" t="n">
         <v>80</v>
       </c>
-      <c r="H13" s="55" t="n">
+      <c r="H13" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I13" s="57"/>
+      <c r="I13" s="58"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5963,18 +5982,18 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="2" sqref="B2 B26 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.4858299595142"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5991902834008"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.5263157894737"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
@@ -5994,13 +6013,13 @@
         <v>108</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>11</v>
@@ -6010,328 +6029,328 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="58" t="s">
+      <c r="A2" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="54" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G2" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H2" s="55" t="n">
+      <c r="H2" s="56" t="n">
         <v>43876</v>
       </c>
       <c r="I2" s="61"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="58" t="s">
+      <c r="A3" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="54" t="s">
         <v>59</v>
       </c>
       <c r="F3" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G3" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H3" s="55" t="n">
+      <c r="H3" s="56" t="n">
         <v>43876</v>
       </c>
       <c r="I3" s="61"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="58" t="s">
+      <c r="A4" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="54" t="s">
         <v>52</v>
       </c>
       <c r="F4" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G4" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H4" s="55" t="n">
+      <c r="H4" s="56" t="n">
         <v>43876</v>
       </c>
       <c r="I4" s="61"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="58" t="s">
+      <c r="A5" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="54" t="s">
         <v>59</v>
       </c>
       <c r="F5" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G5" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H5" s="55" t="n">
+      <c r="H5" s="56" t="n">
         <v>43876</v>
       </c>
       <c r="I5" s="61"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="58" t="s">
+      <c r="A6" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="59" t="s">
         <v>115</v>
-      </c>
-      <c r="E6" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="59" t="s">
-        <v>113</v>
       </c>
       <c r="G6" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H6" s="55" t="n">
+      <c r="H6" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I6" s="54"/>
+      <c r="I6" s="55"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="58" t="s">
+      <c r="A7" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="54" t="s">
         <v>52</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G7" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H7" s="55" t="n">
+      <c r="H7" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I7" s="54"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="58" t="s">
+      <c r="A8" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="54" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G8" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H8" s="55" t="n">
+      <c r="H8" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I8" s="54"/>
+      <c r="I8" s="55"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" s="58" t="s">
+      <c r="C9" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="54" t="s">
         <v>59</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G9" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H9" s="55" t="n">
+      <c r="H9" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I9" s="54"/>
+      <c r="I9" s="55"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D10" s="58" t="s">
+      <c r="C10" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="54" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G10" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H10" s="55" t="n">
+      <c r="H10" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I10" s="54"/>
+      <c r="I10" s="55"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="58" t="s">
+      <c r="C11" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="54" t="s">
         <v>59</v>
       </c>
       <c r="F11" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G11" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H11" s="55" t="n">
+      <c r="H11" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I11" s="54"/>
+      <c r="I11" s="55"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="C12" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="59" t="s">
         <v>115</v>
-      </c>
-      <c r="E12" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="59" t="s">
-        <v>113</v>
       </c>
       <c r="G12" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H12" s="55" t="n">
+      <c r="H12" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I12" s="54"/>
+      <c r="I12" s="55"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="C13" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="54" t="s">
         <v>52</v>
       </c>
       <c r="F13" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G13" s="60" t="n">
         <v>45</v>
       </c>
-      <c r="H13" s="55" t="n">
+      <c r="H13" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="I13" s="54"/>
+      <c r="I13" s="55"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6349,22 +6368,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="2" sqref="B2 B26 B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.7408906882591"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.3076923076923"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="49" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="49" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="49" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="49" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -6384,16 +6403,16 @@
         <v>108</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>48</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H1" s="51" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I1" s="51" t="s">
         <v>11</v>
@@ -6403,305 +6422,219 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="58" t="s">
+      <c r="A2" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="60" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" s="56" t="n">
+        <v>43845</v>
+      </c>
+      <c r="J2" s="62"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="60" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" s="63" t="n">
+        <v>43936</v>
+      </c>
+      <c r="J3" s="62"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E4" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F4" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G4" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="64" t="n">
+        <v>15</v>
+      </c>
+      <c r="I4" s="56" t="n">
+        <v>43845</v>
+      </c>
+      <c r="J4" s="61"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="64" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" s="56" t="n">
+        <v>43845</v>
+      </c>
+      <c r="J5" s="61"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6" s="64" t="n">
+        <v>15</v>
+      </c>
+      <c r="I6" s="56" t="n">
+        <v>43845</v>
+      </c>
+      <c r="J6" s="61"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="62" t="n">
+      <c r="C7" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="64" t="n">
+        <v>10</v>
+      </c>
+      <c r="I7" s="56" t="n">
+        <v>43845</v>
+      </c>
+      <c r="J7" s="61"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="54" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="H8" s="64" t="n">
         <v>15</v>
       </c>
-      <c r="I2" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J2" s="61"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="H3" s="62" t="n">
-        <v>15</v>
-      </c>
-      <c r="I3" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J3" s="61"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="H4" s="62" t="n">
-        <v>15</v>
-      </c>
-      <c r="I4" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J4" s="61"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="H5" s="62" t="n">
-        <v>15</v>
-      </c>
-      <c r="I5" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J5" s="61"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="H6" s="62" t="n">
-        <v>15</v>
-      </c>
-      <c r="I6" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J6" s="54"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="H7" s="62" t="n">
-        <v>15</v>
-      </c>
-      <c r="I7" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J7" s="54"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="H8" s="62" t="n">
-        <v>15</v>
-      </c>
-      <c r="I8" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J8" s="54"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="H9" s="62" t="n">
-        <v>15</v>
-      </c>
-      <c r="I9" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J9" s="54"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B10" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="H10" s="62" t="n">
-        <v>15</v>
-      </c>
-      <c r="I10" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J10" s="54"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="H11" s="62" t="n">
-        <v>15</v>
-      </c>
-      <c r="I11" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J11" s="54"/>
-    </row>
+      <c r="I8" s="56" t="n">
+        <v>43845</v>
+      </c>
+      <c r="J8" s="61"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -6718,19 +6651,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="2" sqref="B2 B26 B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.4534412955466"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.4858299595142"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.0971659919028"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="49" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.1417004048583"/>
@@ -6759,25 +6692,25 @@
         <v>48</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>11</v>
@@ -6787,256 +6720,262 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="58" t="s">
+      <c r="A2" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="54" t="s">
         <v>55</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G2" s="60" t="n">
         <v>80</v>
       </c>
-      <c r="H2" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="I2" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="J2" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="K2" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="L2" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="M2" s="55" t="n">
+      <c r="H2" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="L2" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="56" t="n">
         <v>43876</v>
       </c>
       <c r="N2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="58" t="s">
+      <c r="A3" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="58" t="s">
-        <v>129</v>
+      <c r="E3" s="54" t="s">
+        <v>135</v>
       </c>
       <c r="F3" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G3" s="60" t="n">
         <v>80</v>
       </c>
-      <c r="H3" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="I3" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="J3" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="L3" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="M3" s="55" t="n">
+      <c r="H3" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="K3" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="L3" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="N3" s="58"/>
+      <c r="N3" s="54"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="58" t="s">
+      <c r="A4" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="54" t="s">
         <v>63</v>
       </c>
       <c r="F4" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G4" s="60" t="n">
         <v>80</v>
       </c>
-      <c r="H4" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="I4" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="J4" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="K4" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="L4" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="M4" s="55" t="n">
+      <c r="H4" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="I4" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="L4" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="M4" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="N4" s="58"/>
+      <c r="N4" s="54"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="58" t="s">
+      <c r="A5" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="54" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G5" s="60" t="n">
         <v>80</v>
       </c>
-      <c r="H5" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="I5" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="J5" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="K5" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="L5" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="M5" s="55" t="n">
+      <c r="H5" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="K5" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="M5" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="N5" s="58"/>
+      <c r="N5" s="54"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="58" t="s">
+      <c r="A6" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="E6" s="54" t="s">
         <v>66</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G6" s="60" t="n">
         <v>80</v>
       </c>
-      <c r="H6" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="I6" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="J6" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="L6" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="M6" s="55" t="n">
+      <c r="H6" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="I6" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="J6" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="K6" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="L6" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="M6" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="N6" s="58"/>
+      <c r="N6" s="54"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="58" t="s">
+      <c r="A7" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="54" t="s">
         <v>68</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G7" s="60" t="n">
         <v>80</v>
       </c>
-      <c r="H7" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="I7" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="J7" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="K7" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="L7" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="M7" s="55" t="n">
+      <c r="H7" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="I7" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="J7" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="K7" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="L7" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="M7" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="N7" s="58"/>
+      <c r="N7" s="54"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="54"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="54"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7056,19 +6995,19 @@
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="2" sqref="B2 B26 B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.4858299595142"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0283400809717"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="84.8380566801619"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="91.8016194331984"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -7091,13 +7030,13 @@
         <v>48</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>11</v>
@@ -7107,244 +7046,244 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="58" t="s">
+      <c r="A2" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="58" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>135</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="H2" s="58" t="s">
+      <c r="E2" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="56" t="n">
+        <v>43876</v>
+      </c>
+      <c r="J2" s="62"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="55" t="n">
+      <c r="C3" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="J2" s="63"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="58" t="s">
+      <c r="J3" s="62"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" s="58" t="s">
+      <c r="E4" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" s="56" t="n">
+        <v>43876</v>
+      </c>
+      <c r="J4" s="62"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="G3" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="58" t="s">
+      <c r="B5" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="55" t="n">
+      <c r="C5" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="H5" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="J3" s="63"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="58" t="s">
+      <c r="J5" s="62"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="58" t="s">
-        <v>139</v>
-      </c>
-      <c r="F4" s="58" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="H4" s="58" t="s">
+      <c r="E6" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" s="56" t="n">
+        <v>43876</v>
+      </c>
+      <c r="J6" s="62"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="55" t="n">
+      <c r="C7" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="56" t="n">
         <v>43876</v>
       </c>
-      <c r="J4" s="63"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="F5" s="58" t="s">
-        <v>141</v>
-      </c>
-      <c r="G5" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="H5" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="I5" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J5" s="63"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="G6" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="H6" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="I6" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J6" s="63"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="58" t="s">
-        <v>143</v>
-      </c>
-      <c r="G7" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="H7" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="I7" s="55" t="n">
-        <v>43876</v>
-      </c>
-      <c r="J7" s="63"/>
+      <c r="J7" s="62"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="58"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="63"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="58"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="63"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="58"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="63"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="58"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="63"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="62"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="58"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="63"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="62"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7365,7 +7304,7 @@
   <dimension ref="1:40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K55" activeCellId="0" sqref="K55"/>
+      <selection pane="topLeft" activeCell="K55" activeCellId="2" sqref="B2 B26 K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -7373,19 +7312,19 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="6" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="6" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="6" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="28.2793522267206"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="6" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="45.417004048583"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="6" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="6" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="6" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="6" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="6" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="6" width="9.10526315789474"/>
@@ -9483,7 +9422,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>40</v>
@@ -10099,7 +10038,7 @@
         <v>78</v>
       </c>
       <c r="K20" s="31" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="L20" s="31"/>
       <c r="M20" s="31" t="s">
@@ -10141,7 +10080,7 @@
         <v>79</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="L21" s="32" t="s">
         <v>54</v>
@@ -10916,7 +10855,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="2" sqref="B2 B26 B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -10924,248 +10863,248 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="6" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="9" min="2" style="6" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="10" style="6" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="64" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="64" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="65" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="65" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="6" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="65" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="A1" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
       <c r="I1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="66" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="67"/>
+      <c r="B2" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
-      <c r="B3" s="66" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="B3" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
       <c r="I4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="68" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
+      <c r="A5" s="69" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
       <c r="I5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="70" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" s="70" t="s">
+      <c r="A6" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="70" t="s">
+      <c r="F6" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="70" t="s">
+      <c r="G6" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="70" t="s">
+      <c r="H6" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="70" t="s">
+      <c r="I6" s="71" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="71" t="n">
+      <c r="A7" s="72" t="n">
         <v>8</v>
       </c>
-      <c r="B7" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="72" t="s">
-        <v>153</v>
-      </c>
-      <c r="D7" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="73" t="s">
-        <v>154</v>
-      </c>
-      <c r="F7" s="73" t="s">
-        <v>155</v>
-      </c>
-      <c r="G7" s="73" t="s">
-        <v>156</v>
-      </c>
-      <c r="H7" s="73" t="s">
+      <c r="B7" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="I7" s="73" t="s">
+      <c r="C7" s="73" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" s="74" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="72" t="n">
+        <v>9</v>
+      </c>
+      <c r="B8" s="73" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="71" t="n">
-        <v>9</v>
-      </c>
-      <c r="B8" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="72" t="s">
-        <v>153</v>
-      </c>
-      <c r="D8" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="73" t="s">
-        <v>154</v>
-      </c>
-      <c r="F8" s="73" t="s">
-        <v>155</v>
-      </c>
-      <c r="G8" s="73" t="s">
-        <v>156</v>
-      </c>
-      <c r="H8" s="73" t="s">
+      <c r="C8" s="73" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="H8" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="I8" s="74" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="72" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="I8" s="73" t="s">
+      <c r="C9" s="73" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="G9" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="H9" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="I9" s="74" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="72" t="n">
+        <v>11</v>
+      </c>
+      <c r="B10" s="73" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="71" t="n">
-        <v>10</v>
-      </c>
-      <c r="B9" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="C9" s="72" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="73" t="s">
-        <v>154</v>
-      </c>
-      <c r="F9" s="73" t="s">
-        <v>155</v>
-      </c>
-      <c r="G9" s="73" t="s">
-        <v>156</v>
-      </c>
-      <c r="H9" s="73" t="s">
+      <c r="C10" s="73" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="F10" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="G10" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="H10" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="I10" s="74" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="72" t="n">
+        <v>12</v>
+      </c>
+      <c r="B11" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="I9" s="73" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="71" t="n">
-        <v>11</v>
-      </c>
-      <c r="B10" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="C10" s="72" t="s">
-        <v>153</v>
-      </c>
-      <c r="D10" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="E10" s="73" t="s">
-        <v>154</v>
-      </c>
-      <c r="F10" s="73" t="s">
-        <v>155</v>
-      </c>
-      <c r="G10" s="73" t="s">
-        <v>156</v>
-      </c>
-      <c r="H10" s="73" t="s">
-        <v>157</v>
-      </c>
-      <c r="I10" s="73" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="71" t="n">
-        <v>12</v>
-      </c>
-      <c r="B11" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="72" t="s">
-        <v>153</v>
-      </c>
-      <c r="D11" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="E11" s="73" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" s="73" t="s">
-        <v>155</v>
-      </c>
-      <c r="G11" s="73" t="s">
-        <v>156</v>
-      </c>
-      <c r="H11" s="73" t="s">
-        <v>157</v>
-      </c>
-      <c r="I11" s="73" t="s">
-        <v>157</v>
+      <c r="C11" s="73" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="G11" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="H11" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="I11" s="74" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11176,105 +11115,105 @@
       <c r="E12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="70" t="s">
-        <v>151</v>
-      </c>
-      <c r="B13" s="70" t="s">
+      <c r="A13" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="70" t="s">
+      <c r="E13" s="71" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="71" t="n">
+      <c r="A14" s="72" t="n">
         <v>8</v>
       </c>
-      <c r="B14" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="C14" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="D14" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="E14" s="72" t="s">
-        <v>154</v>
+      <c r="B14" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="73" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="71" t="n">
+      <c r="A15" s="72" t="n">
         <v>9</v>
       </c>
-      <c r="B15" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="C15" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="D15" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="E15" s="72" t="s">
-        <v>154</v>
+      <c r="B15" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15" s="73" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="71" t="n">
+      <c r="A16" s="72" t="n">
         <v>10</v>
       </c>
-      <c r="B16" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="C16" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="D16" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="E16" s="72" t="s">
-        <v>154</v>
+      <c r="B16" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="73" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="71" t="n">
+      <c r="A17" s="72" t="n">
         <v>11</v>
       </c>
-      <c r="B17" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="C17" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="D17" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="E17" s="72" t="s">
-        <v>154</v>
+      <c r="B17" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="C17" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" s="73" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="71" t="n">
+      <c r="A18" s="72" t="n">
         <v>12</v>
       </c>
-      <c r="B18" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="C18" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="D18" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="E18" s="72" t="s">
-        <v>154</v>
+      <c r="B18" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="E18" s="73" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11284,82 +11223,82 @@
       <c r="D19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="68" t="s">
-        <v>159</v>
+      <c r="A20" s="69" t="s">
+        <v>164</v>
       </c>
       <c r="B20" s="0"/>
       <c r="C20" s="0"/>
       <c r="D20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="70" t="s">
-        <v>151</v>
-      </c>
-      <c r="B21" s="70" t="s">
+      <c r="A21" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="70" t="s">
+      <c r="C21" s="71" t="s">
         <v>79</v>
       </c>
       <c r="D21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="71" t="n">
+      <c r="A22" s="72" t="n">
         <v>8</v>
       </c>
-      <c r="B22" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C22" s="72" t="s">
-        <v>160</v>
+      <c r="B22" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="73" t="s">
+        <v>165</v>
       </c>
       <c r="D22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="71" t="n">
+      <c r="A23" s="72" t="n">
         <v>9</v>
       </c>
-      <c r="B23" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C23" s="72" t="s">
-        <v>160</v>
+      <c r="B23" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="73" t="s">
+        <v>165</v>
       </c>
       <c r="D23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="71" t="n">
+      <c r="A24" s="72" t="n">
         <v>10</v>
       </c>
-      <c r="B24" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" s="72" t="s">
-        <v>160</v>
+      <c r="B24" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="73" t="s">
+        <v>165</v>
       </c>
       <c r="D24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="71" t="n">
+      <c r="A25" s="72" t="n">
         <v>11</v>
       </c>
-      <c r="B25" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C25" s="72" t="s">
-        <v>160</v>
+      <c r="B25" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="73" t="s">
+        <v>165</v>
       </c>
       <c r="D25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="71" t="n">
+      <c r="A26" s="72" t="n">
         <v>12</v>
       </c>
-      <c r="B26" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C26" s="72" t="s">
-        <v>160</v>
+      <c r="B26" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="73" t="s">
+        <v>165</v>
       </c>
       <c r="D26" s="0"/>
     </row>
@@ -11370,7 +11309,7 @@
       <c r="D27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="69" t="s">
         <v>80</v>
       </c>
       <c r="B28" s="0"/>
@@ -11378,87 +11317,87 @@
       <c r="D28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="70" t="s">
-        <v>151</v>
-      </c>
-      <c r="B29" s="70" t="s">
-        <v>161</v>
-      </c>
-      <c r="C29" s="70" t="s">
+      <c r="A29" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="70" t="s">
+      <c r="D29" s="71" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="71" t="n">
+      <c r="A30" s="72" t="n">
         <v>8</v>
       </c>
-      <c r="B30" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D30" s="72" t="s">
-        <v>153</v>
+      <c r="B30" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="73" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="71" t="n">
+      <c r="A31" s="72" t="n">
         <v>9</v>
       </c>
-      <c r="B31" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C31" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D31" s="72" t="s">
-        <v>153</v>
+      <c r="B31" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="73" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="71" t="n">
+      <c r="A32" s="72" t="n">
         <v>10</v>
       </c>
-      <c r="B32" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D32" s="72" t="s">
-        <v>153</v>
+      <c r="B32" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="73" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="71" t="n">
+      <c r="A33" s="72" t="n">
         <v>11</v>
       </c>
-      <c r="B33" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C33" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D33" s="72" t="s">
-        <v>153</v>
+      <c r="B33" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="73" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="71" t="n">
+      <c r="A34" s="72" t="n">
         <v>12</v>
       </c>
-      <c r="B34" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C34" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D34" s="72" t="s">
-        <v>153</v>
+      <c r="B34" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="73" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11468,95 +11407,95 @@
       <c r="D35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="68" t="s">
-        <v>162</v>
+      <c r="A36" s="69" t="s">
+        <v>167</v>
       </c>
       <c r="B36" s="0"/>
       <c r="C36" s="0"/>
       <c r="D36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="70" t="s">
-        <v>151</v>
-      </c>
-      <c r="B37" s="70" t="s">
-        <v>163</v>
-      </c>
-      <c r="C37" s="70" t="s">
-        <v>164</v>
-      </c>
-      <c r="D37" s="70" t="s">
-        <v>165</v>
+      <c r="A37" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" s="71" t="s">
+        <v>168</v>
+      </c>
+      <c r="C37" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="D37" s="71" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="71" t="n">
+      <c r="A38" s="72" t="n">
         <v>8</v>
       </c>
-      <c r="B38" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="C38" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D38" s="72" t="s">
-        <v>154</v>
+      <c r="B38" s="73" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="73" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="71" t="n">
+      <c r="A39" s="72" t="n">
         <v>9</v>
       </c>
-      <c r="B39" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" s="72" t="s">
-        <v>154</v>
+      <c r="B39" s="73" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="73" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="71" t="n">
+      <c r="A40" s="72" t="n">
         <v>10</v>
       </c>
-      <c r="B40" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="C40" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" s="72" t="s">
-        <v>154</v>
+      <c r="B40" s="73" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" s="73" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="71" t="n">
+      <c r="A41" s="72" t="n">
         <v>11</v>
       </c>
-      <c r="B41" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D41" s="72" t="s">
-        <v>154</v>
+      <c r="B41" s="73" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="73" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="71" t="n">
+      <c r="A42" s="72" t="n">
         <v>12</v>
       </c>
-      <c r="B42" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="C42" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D42" s="72" t="s">
-        <v>154</v>
+      <c r="B42" s="73" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" s="73" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>